<commit_message>
Play around in playground, update fixture Investigation file
</commit_message>
<xml_diff>
--- a/tests/ArcGraphModel.IO.Tests/Fixtures/isa.investigation.xlsx
+++ b/tests/ArcGraphModel.IO.Tests/Fixtures/isa.investigation.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/630acb9a9506da97/CSB-Stuff/NFDI/testARC30/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\ArcGraphModel\tests\ArcGraphModel.IO.Tests\Fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_8EF33D3ED672484A984217D33883018CD10D0B48" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B1C9822-F11E-4AB6-9D10-88DED0DE17A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84808EE5-2048-46A2-ACFE-172AF51E66E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_investigation" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="116">
   <si>
     <t>ONTOLOGY SOURCE REFERENCE</t>
   </si>
@@ -122,9 +123,6 @@
     <t>Oliver</t>
   </si>
   <si>
-    <t>Schnevin</t>
-  </si>
-  <si>
     <t>Investigation Person Mid Initials</t>
   </si>
   <si>
@@ -375,6 +373,15 @@
   </si>
   <si>
     <t>Comment[&lt;Investigation Person lol&gt;]</t>
+  </si>
+  <si>
+    <t>müller</t>
+  </si>
+  <si>
+    <t>oih</t>
+  </si>
+  <si>
+    <t>andreas</t>
   </si>
 </sst>
 </file>
@@ -916,10 +923,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1219,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,27 +1330,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1357,171 +1360,177 @@
       <c r="C21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
       <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>30</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>35</v>
       </c>
-      <c r="B25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>36</v>
       </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>37</v>
       </c>
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
         <v>38</v>
       </c>
-      <c r="B28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="B29" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>41</v>
       </c>
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>42</v>
       </c>
-      <c r="B31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
         <v>43</v>
-      </c>
-      <c r="B32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B33" t="s">
         <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
         <v>46</v>
-      </c>
-      <c r="B35" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
         <v>48</v>
-      </c>
-      <c r="B36" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" t="s">
         <v>50</v>
-      </c>
-      <c r="B37" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
@@ -1529,7 +1538,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
         <v>13</v>
@@ -1537,105 +1546,105 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" t="s">
         <v>54</v>
-      </c>
-      <c r="B40" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B59" t="s">
         <v>13</v>
@@ -1646,7 +1655,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B60" t="s">
         <v>13</v>
@@ -1657,7 +1666,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
         <v>13</v>
@@ -1668,7 +1677,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
         <v>13</v>
@@ -1679,7 +1688,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B63" t="s">
         <v>13</v>
@@ -1690,7 +1699,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B64" t="s">
         <v>13</v>
@@ -1701,7 +1710,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B65" t="s">
         <v>13</v>
@@ -1712,101 +1721,101 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>80</v>
+      </c>
+      <c r="B66" t="s">
         <v>81</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>82</v>
-      </c>
-      <c r="C66" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>99</v>
+      </c>
+      <c r="B83" t="s">
         <v>100</v>
-      </c>
-      <c r="B83" t="s">
-        <v>101</v>
       </c>
       <c r="C83" t="s">
         <v>13</v>
@@ -1814,18 +1823,18 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" t="s">
+        <v>13</v>
+      </c>
+      <c r="C84" t="s">
         <v>102</v>
-      </c>
-      <c r="B84" t="s">
-        <v>13</v>
-      </c>
-      <c r="C84" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B85" t="s">
         <v>13</v>
@@ -1836,7 +1845,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B86" t="s">
         <v>13</v>
@@ -1847,7 +1856,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B87" t="s">
         <v>13</v>
@@ -1858,7 +1867,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B88" t="s">
         <v>13</v>
@@ -1869,7 +1878,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B89" t="s">
         <v>13</v>
@@ -1880,7 +1889,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B90" t="s">
         <v>13</v>
@@ -1891,7 +1900,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B91" t="s">
         <v>13</v>
@@ -1902,7 +1911,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B92" t="s">
         <v>13</v>
@@ -1913,13 +1922,38 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B93" t="s">
         <v>13</v>
       </c>
       <c r="C93" t="s">
         <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4D0F7B-7CB1-4B7D-BB14-8880F01D8D52}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" activeCellId="1" sqref="A1 I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>